<commit_message>
wip - documents prior to bifunction
</commit_message>
<xml_diff>
--- a/owlcms/src/main/resources/templates/cards/Card-A4.xlsx
+++ b/owlcms/src/main/resources/templates/cards/Card-A4.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lamyj\git\owlcms4\owlcms\local\templates\cards\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lamyj\git\owlcms4\owlcms\src\main\resources\templates\cards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0840BCF-4E41-49CF-8309-56EFA4F04506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFC35993-B287-43EC-A960-03E6BD1DF9A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1095" yWindow="3255" windowWidth="19590" windowHeight="12015" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -59,15 +59,32 @@
         </r>
       </text>
     </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{DD5D7428-31E2-4FD5-9552-E92A8463D510}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Aptos Narrow"/>
+            <family val="2"/>
+          </rPr>
+          <t>jx:area(
+  lastCell="I24"
+)
+jx:each(
+  items="athletes"
+  var="athlete"
+  lastCell="I24"
+)</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="34">
-  <si>
-    <t>${session.localizedStartHour}</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="31">
   <si>
     <t>${competition.competitionName} / ${competition.competitionCity}</t>
   </si>
@@ -102,18 +119,9 @@
     <t>${t.get("Card.birthDate")}</t>
   </si>
   <si>
-    <t>${l.category}</t>
-  </si>
-  <si>
-    <t>${l.formattedBirth}</t>
-  </si>
-  <si>
     <t>${t.get("Card.startNumber")}</t>
   </si>
   <si>
-    <t>${t.get("Group")}: ${session.name}</t>
-  </si>
-  <si>
     <t>${t.get("Card.entryTotal")}</t>
   </si>
   <si>
@@ -141,9 +149,6 @@
     <t>${athlete.ageGroup.code}</t>
   </si>
   <si>
-    <t>${t.get("Card.category")}${t.get("AgeGroup")</t>
-  </si>
-  <si>
     <t>${t.get("Total")}</t>
   </si>
   <si>
@@ -165,7 +170,13 @@
     <t>${t.get("Card.RequiredCJ")}</t>
   </si>
   <si>
-    <t>${session.localizedStartDay}</t>
+    <t>${t.get("Group")}: ${athlete.group}</t>
+  </si>
+  <si>
+    <t>${athlete.group.localizedStartDay}</t>
+  </si>
+  <si>
+    <t>${athlete.group.localizedStartHour}</t>
   </si>
 </sst>
 </file>
@@ -623,7 +634,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
@@ -651,17 +662,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -811,16 +816,10 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1172,10 +1171,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:D9"/>
+      <selection activeCell="B2" sqref="B2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1193,238 +1192,238 @@
   <sheetData>
     <row r="1" spans="1:10" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="B1" s="1"/>
-      <c r="C1" s="17" t="s">
-        <v>33</v>
+      <c r="C1" s="15" t="s">
+        <v>29</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="G1" s="1"/>
-      <c r="H1" s="17" t="s">
-        <v>33</v>
+      <c r="H1" s="15" t="s">
+        <v>29</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="41"/>
-      <c r="F2" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="40"/>
-      <c r="I2" s="41"/>
+      <c r="A2" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="38"/>
+      <c r="D2" s="39"/>
+      <c r="F2" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="38"/>
+      <c r="I2" s="39"/>
     </row>
     <row r="3" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
-      <c r="B3" s="42" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="43"/>
-      <c r="D3" s="44"/>
+      <c r="B3" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="41"/>
+      <c r="D3" s="42"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="42" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="43"/>
-      <c r="I3" s="44"/>
+      <c r="G3" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="41"/>
+      <c r="I3" s="42"/>
     </row>
     <row r="4" spans="1:10" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
-      <c r="B4" s="45" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="46"/>
-      <c r="D4" s="47"/>
+      <c r="B4" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="44"/>
+      <c r="D4" s="45"/>
       <c r="F4" s="2"/>
-      <c r="G4" s="57" t="s">
-        <v>1</v>
-      </c>
-      <c r="H4" s="58"/>
-      <c r="I4" s="59"/>
+      <c r="G4" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4" s="56"/>
+      <c r="I4" s="57"/>
     </row>
     <row r="5" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="53" t="s">
+      <c r="A5" s="51" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="52"/>
+      <c r="C5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="54"/>
-      <c r="C5" s="10" t="s">
+      <c r="D5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="53" t="s">
+      <c r="F5" s="51" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="52"/>
+      <c r="H5" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="54"/>
-      <c r="H5" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="6" spans="1:10" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="55" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="56"/>
-      <c r="C6" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="28"/>
-      <c r="F6" s="55" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6" s="56"/>
-      <c r="H6" s="12" t="s">
+      <c r="A6" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="54"/>
+      <c r="C6" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="12" t="s">
+      <c r="E6" s="26"/>
+      <c r="F6" s="53" t="s">
         <v>4</v>
+      </c>
+      <c r="G6" s="54"/>
+      <c r="H6" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="12"/>
+      <c r="H7" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="35" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="49" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="50"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="16"/>
+      <c r="F8" s="58" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="59"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="33"/>
+    </row>
+    <row r="9" spans="1:10" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="47"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="48"/>
+      <c r="F9" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="61"/>
+      <c r="H9" s="61"/>
+      <c r="I9" s="62"/>
+    </row>
+    <row r="10" spans="1:10" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="63">
+        <v>1</v>
+      </c>
+      <c r="B10" s="64"/>
+      <c r="C10" s="13">
+        <v>2</v>
+      </c>
+      <c r="D10" s="14">
+        <v>3</v>
+      </c>
+      <c r="F10" s="63">
+        <v>1</v>
+      </c>
+      <c r="G10" s="64"/>
+      <c r="H10" s="13">
+        <v>2</v>
+      </c>
+      <c r="I10" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="65"/>
+      <c r="B11" s="66"/>
+      <c r="C11" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7" s="13"/>
-      <c r="H7" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="I7" s="37" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="51" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="52"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="18"/>
-      <c r="F8" s="60" t="s">
-        <v>30</v>
-      </c>
-      <c r="G8" s="61"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="35"/>
-    </row>
-    <row r="9" spans="1:10" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="49"/>
-      <c r="C9" s="49"/>
-      <c r="D9" s="50"/>
-      <c r="F9" s="62" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" s="63"/>
-      <c r="H9" s="63"/>
-      <c r="I9" s="64"/>
-    </row>
-    <row r="10" spans="1:10" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="66">
-        <v>1</v>
-      </c>
-      <c r="B10" s="67"/>
-      <c r="C10" s="15">
-        <v>2</v>
-      </c>
-      <c r="D10" s="16">
-        <v>3</v>
-      </c>
-      <c r="F10" s="66">
-        <v>1</v>
-      </c>
-      <c r="G10" s="67"/>
-      <c r="H10" s="15">
-        <v>2</v>
-      </c>
-      <c r="I10" s="16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="69"/>
-      <c r="B11" s="70"/>
-      <c r="C11" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="69"/>
-      <c r="G11" s="70"/>
-      <c r="H11" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="I11" s="32" t="s">
-        <v>20</v>
+      <c r="D11" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="65"/>
+      <c r="G11" s="66"/>
+      <c r="H11" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" s="30" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="29.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="71"/>
-      <c r="B12" s="72"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="34"/>
-      <c r="F12" s="71"/>
-      <c r="G12" s="72"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="34"/>
+      <c r="A12" s="67"/>
+      <c r="B12" s="68"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="32"/>
+      <c r="F12" s="67"/>
+      <c r="G12" s="68"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="32"/>
     </row>
     <row r="13" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G13" s="4"/>
       <c r="H13" s="7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1438,57 +1437,57 @@
       <c r="I14" s="6"/>
     </row>
     <row r="15" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="22"/>
-      <c r="C15" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="F15" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="G15" s="22"/>
-      <c r="H15" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="I15" s="23" t="s">
-        <v>2</v>
+      <c r="A15" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="20"/>
+      <c r="C15" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" s="20"/>
+      <c r="H15" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="I15" s="21" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="29.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="19"/>
-      <c r="B16" s="20"/>
+      <c r="A16" s="17"/>
+      <c r="B16" s="18"/>
       <c r="C16" s="5"/>
       <c r="D16" s="6"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="20"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="18"/>
       <c r="H16" s="5"/>
       <c r="I16" s="6"/>
     </row>
     <row r="17" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G17" s="4"/>
       <c r="H17" s="7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1502,57 +1501,57 @@
       <c r="I18" s="6"/>
     </row>
     <row r="19" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="B19" s="22"/>
-      <c r="C19" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="D19" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="F19" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="G19" s="22"/>
-      <c r="H19" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="I19" s="23" t="s">
-        <v>2</v>
+      <c r="A19" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="20"/>
+      <c r="C19" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" s="20"/>
+      <c r="H19" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="I19" s="21" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="29.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="19"/>
-      <c r="B20" s="20"/>
+      <c r="A20" s="17"/>
+      <c r="B20" s="18"/>
       <c r="C20" s="5"/>
       <c r="D20" s="6"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="20"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="18"/>
       <c r="H20" s="5"/>
       <c r="I20" s="6"/>
     </row>
     <row r="21" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G21" s="4"/>
       <c r="H21" s="7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1566,35 +1565,35 @@
       <c r="I22" s="6"/>
     </row>
     <row r="23" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="B23" s="22"/>
-      <c r="C23" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="D23" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="F23" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="G23" s="22"/>
-      <c r="H23" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="I23" s="23" t="s">
-        <v>2</v>
+      <c r="A23" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="20"/>
+      <c r="C23" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F23" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="G23" s="20"/>
+      <c r="H23" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="I23" s="21" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="29.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="19"/>
-      <c r="B24" s="20"/>
-      <c r="C24" s="19"/>
+      <c r="A24" s="17"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="17"/>
       <c r="D24" s="9"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="19"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="17"/>
       <c r="I24" s="9"/>
     </row>
     <row r="25" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1607,60 +1606,12 @@
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
     </row>
-    <row r="26" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="65"/>
-      <c r="B26" s="65"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="H26" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="I26" s="3"/>
-    </row>
-    <row r="27" spans="1:9" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="68"/>
-      <c r="B27" s="68"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="68"/>
-      <c r="E27" s="68"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="H27" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="I27" s="11"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F30" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="G30" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="F31" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="G31" s="14" t="s">
-        <v>13</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="A26:B26"/>
+  <mergeCells count="18">
     <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A27:B27"/>
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="A11:B12"/>
     <mergeCell ref="F11:G12"/>
-    <mergeCell ref="D27:E27"/>
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="G3:I3"/>
     <mergeCell ref="G4:I4"/>

</xml_diff>